<commit_message>
Broken Changes: Need to fix issue with sql command not found
</commit_message>
<xml_diff>
--- a/Excel Files/Theater Table.xlsx
+++ b/Excel Files/Theater Table.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\odonn\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosen\source\repos\560FinalProject\Excel Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B8B4AE2B-0037-407D-BED2-0D5E0C108A05}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D4D942D-3BBB-40A5-9BAC-A4B3AF3D6DB4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-16320" yWindow="2175" windowWidth="16440" windowHeight="28440" xr2:uid="{0C57311F-6FFE-49F3-B544-3D4EF0A82D3B}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11385" xr2:uid="{0C57311F-6FFE-49F3-B544-3D4EF0A82D3B}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -38,9 +38,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
   <si>
-    <t>1. AMC Empire 25</t>
-  </si>
-  <si>
     <t>1000 W Olympic Blvd, Los Angeles, CA 90015</t>
   </si>
   <si>
@@ -56,15 +53,9 @@
     <t>4. ArcLight Hollywood</t>
   </si>
   <si>
-    <t>5. Cinemark Tinseltown 20 and XD</t>
-  </si>
-  <si>
     <t>7. Landmark's Magnolia Theatre</t>
   </si>
   <si>
-    <t>6. Cinemark Playa Vista and XD</t>
-  </si>
-  <si>
     <t xml:space="preserve">9. Angelika Film Center &amp; Café </t>
   </si>
   <si>
@@ -156,6 +147,15 @@
   </si>
   <si>
     <t>5904 York Rd, Baltimore, MD 21212</t>
+  </si>
+  <si>
+    <t>1. AMC Empire</t>
+  </si>
+  <si>
+    <t>5. Cinemark Tinseltown</t>
+  </si>
+  <si>
+    <t>6. Cinemark Playa Vista</t>
   </si>
 </sst>
 </file>
@@ -536,7 +536,7 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -548,10 +548,10 @@
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
-        <v>0</v>
+        <v>37</v>
       </c>
       <c r="B1" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C1">
         <v>12</v>
@@ -559,10 +559,10 @@
     </row>
     <row r="2" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2">
         <v>18</v>
@@ -570,10 +570,10 @@
     </row>
     <row r="3" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C3">
         <v>8</v>
@@ -581,10 +581,10 @@
     </row>
     <row r="4" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>10</v>
@@ -592,10 +592,10 @@
     </row>
     <row r="5" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>6</v>
+        <v>38</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="C5">
         <v>16</v>
@@ -603,10 +603,10 @@
     </row>
     <row r="6" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="C6">
         <v>6</v>
@@ -614,10 +614,10 @@
     </row>
     <row r="7" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C7">
         <v>12</v>
@@ -625,10 +625,10 @@
     </row>
     <row r="8" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="C8">
         <v>10</v>
@@ -636,10 +636,10 @@
     </row>
     <row r="9" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B9" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="C9">
         <v>8</v>
@@ -647,10 +647,10 @@
     </row>
     <row r="10" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10">
         <v>6</v>
@@ -658,10 +658,10 @@
     </row>
     <row r="11" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11">
         <v>12</v>
@@ -669,10 +669,10 @@
     </row>
     <row r="12" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12">
         <v>8</v>
@@ -680,10 +680,10 @@
     </row>
     <row r="13" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13">
         <v>14</v>
@@ -691,10 +691,10 @@
     </row>
     <row r="14" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14">
         <v>6</v>
@@ -702,10 +702,10 @@
     </row>
     <row r="15" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15">
         <v>4</v>
@@ -713,10 +713,10 @@
     </row>
     <row r="16" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C16">
         <v>12</v>
@@ -724,10 +724,10 @@
     </row>
     <row r="17" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="C17">
         <v>10</v>
@@ -735,10 +735,10 @@
     </row>
     <row r="18" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C18">
         <v>10</v>
@@ -746,10 +746,10 @@
     </row>
     <row r="19" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C19">
         <v>6</v>
@@ -757,10 +757,10 @@
     </row>
     <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="C20">
         <v>8</v>

</xml_diff>